<commit_message>
se agrega umbrales criterio de conectividad
</commit_message>
<xml_diff>
--- a/data/config_criteria.xlsx
+++ b/data/config_criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCAD\development\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mcad-0.1.3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CA3200-3C37-4CB1-8403-9724AF9DBC59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997BA7F7-E241-442C-B6C7-DE11AA962B79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="0" windowWidth="36795" windowHeight="16200" firstSheet="1" activeTab="3" xr2:uid="{C442B060-15DE-4315-A6CD-A4F0FD43729D}"/>
+    <workbookView xWindow="14385" yWindow="4140" windowWidth="13530" windowHeight="6000" firstSheet="2" activeTab="5" xr2:uid="{C442B060-15DE-4315-A6CD-A4F0FD43729D}"/>
   </bookViews>
   <sheets>
     <sheet name="ZH_Areas" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Rareza_Criterio_2" sheetId="5" r:id="rId3"/>
     <sheet name="Representatividad" sheetId="6" r:id="rId4"/>
     <sheet name="Especies_Sensibles" sheetId="7" r:id="rId5"/>
+    <sheet name="Conectividad" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ZH_Areas!$A$1:$E$39</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>AH</t>
   </si>
@@ -266,14 +267,30 @@
   </si>
   <si>
     <t>Alta presencia</t>
+  </si>
+  <si>
+    <t>Conectividad</t>
+  </si>
+  <si>
+    <t>Muy Alta</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Muy Baja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -338,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -364,6 +381,10 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1465,7 +1486,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A82D64F-D4B5-4C13-8737-102CAB9C0165}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -1477,7 +1498,7 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -1485,7 +1506,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1493,7 +1514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1501,7 +1522,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -1509,7 +1530,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -1517,7 +1538,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
@@ -1525,10 +1546,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
     </row>
-    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1538,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A113D804-2D9B-4B44-A65B-AB32A3A667E2}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -1644,7 +1664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D186ED5-DDDE-40B4-9C78-6E0B54B1066F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1712,4 +1734,110 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743B96DB-2EE2-4233-85AE-499F37CC13D4}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="16">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="13">
+        <f>0.5/100</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C5" s="13">
+        <f>+B4</f>
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <f>+B5</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>